<commit_message>
Just doing some note calculations
</commit_message>
<xml_diff>
--- a/documentation/b/cv-notes.xlsx
+++ b/documentation/b/cv-notes.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15100" yWindow="5080" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="100">
   <si>
     <t>Note: The data my calculations are based on are based on a spreadsheet from http://obsoletetechnology.wordpress.com/projects/midi-cvgate-converter/</t>
   </si>
@@ -298,13 +298,34 @@
   </si>
   <si>
     <t>Error Cents</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -316,6 +337,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -338,8 +375,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -354,7 +393,9 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -684,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J67"/>
+  <dimension ref="A2:K67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -695,12 +736,12 @@
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1">
+    <row r="5" spans="1:11" s="2" customFormat="1">
       <c r="A5" s="2" t="s">
         <v>86</v>
       </c>
@@ -726,7 +767,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>-57</v>
       </c>
@@ -745,11 +786,11 @@
         <v>12</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" ref="F6:F67" si="2">(1/12)*(E15-21)</f>
+        <f>(1/12)*(E6-12)</f>
         <v>0</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" ref="G6:G67" si="3">ROUND((F6/1.25)*1000,0)</f>
+        <f t="shared" ref="G6:G67" si="2">ROUND((F6/1.25)*1000,0)</f>
         <v>0</v>
       </c>
       <c r="H6" s="3" t="str">
@@ -757,12 +798,15 @@
         <v>000</v>
       </c>
       <c r="I6" s="3">
-        <f t="shared" ref="I6:I67" si="4">G6-(F6/1.25)*1000</f>
+        <f t="shared" ref="I6:I67" si="3">G6-(F6/1.25)*1000</f>
         <v>0</v>
       </c>
       <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>-56</v>
       </c>
@@ -781,11 +825,11 @@
         <v>13</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="2"/>
+        <f>(1/12)*(E7-12)</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>67</v>
       </c>
       <c r="H7" s="3" t="str">
@@ -793,7 +837,7 @@
         <v>043</v>
       </c>
       <c r="I7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.3333333333333286</v>
       </c>
       <c r="J7" s="5">
@@ -801,7 +845,7 @@
         <v>4.9751243781093824E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>-55</v>
       </c>
@@ -820,27 +864,30 @@
         <v>14</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="2"/>
+        <f>(1/12)*(E8-12)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>133</v>
       </c>
       <c r="H8" s="3" t="str">
-        <f t="shared" ref="H8:H67" si="5">DEC2HEX(G8,3)</f>
+        <f t="shared" ref="H8:H67" si="4">DEC2HEX(G8,3)</f>
         <v>085</v>
       </c>
       <c r="I8" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333334281</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" ref="J8:J67" si="6">I8/G8</f>
+        <f t="shared" ref="J8:J67" si="5">I8/G8</f>
         <v>-2.5062656641604724E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>-54</v>
       </c>
@@ -859,27 +906,27 @@
         <v>15</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F9:F67" si="6">(1/12)*(E9-12)</f>
         <v>0.25</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="H9" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0C8</v>
       </c>
       <c r="I9" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J9" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>-53</v>
       </c>
@@ -898,27 +945,30 @@
         <v>16</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>267</v>
       </c>
       <c r="H10" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>10B</v>
       </c>
       <c r="I10" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333331439</v>
       </c>
       <c r="J10" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1.2484394506865708E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>-52</v>
       </c>
@@ -937,27 +987,30 @@
         <v>17</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.41666666666666663</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>333</v>
       </c>
       <c r="H11" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>14D</v>
       </c>
       <c r="I11" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333331439</v>
       </c>
       <c r="J11" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1.0010010010009442E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>-51</v>
       </c>
@@ -976,27 +1029,27 @@
         <v>18</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>400</v>
       </c>
       <c r="H12" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>190</v>
       </c>
       <c r="I12" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J12" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="1">
         <v>-50</v>
       </c>
@@ -1015,27 +1068,30 @@
         <v>19</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.58333333333333326</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>467</v>
       </c>
       <c r="H13" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1D3</v>
       </c>
       <c r="I13" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333337123</v>
       </c>
       <c r="J13" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>7.1377587437552721E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
         <v>-49</v>
       </c>
@@ -1054,27 +1110,27 @@
         <v>20</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>533</v>
       </c>
       <c r="H14" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>215</v>
       </c>
       <c r="I14" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333337123</v>
       </c>
       <c r="J14" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-6.2539086929337944E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" s="1">
         <v>-48</v>
       </c>
@@ -1093,27 +1149,30 @@
         <v>21</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.75</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>600</v>
       </c>
       <c r="H15" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>258</v>
       </c>
       <c r="I15" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="1">
         <v>-47</v>
       </c>
@@ -1132,27 +1191,27 @@
         <v>22</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.83333333333333326</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>667</v>
       </c>
       <c r="H16" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>29B</v>
       </c>
       <c r="I16" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333337123</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4.9975012493758803E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11">
       <c r="A17" s="1">
         <v>-46</v>
       </c>
@@ -1171,27 +1230,30 @@
         <v>23</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.91666666666666663</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>733</v>
       </c>
       <c r="H17" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2DD</v>
       </c>
       <c r="I17" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333325754</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-4.5475216007265695E-4</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="1">
         <v>-45</v>
       </c>
@@ -1210,27 +1272,30 @@
         <v>24</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>800</v>
       </c>
       <c r="H18" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>320</v>
       </c>
       <c r="I18" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1">
         <v>-44</v>
       </c>
@@ -1249,27 +1314,27 @@
         <v>25</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.0833333333333333</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>867</v>
       </c>
       <c r="H19" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>363</v>
       </c>
       <c r="I19" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333337123</v>
       </c>
       <c r="J19" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3.8446751249523786E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:11">
       <c r="A20" s="1">
         <v>-43</v>
       </c>
@@ -1288,27 +1353,30 @@
         <v>26</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.1666666666666665</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>933</v>
       </c>
       <c r="H20" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3A5</v>
       </c>
       <c r="I20" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333325754</v>
       </c>
       <c r="J20" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-3.5727045373339501E-4</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="1">
         <v>-42</v>
       </c>
@@ -1327,27 +1395,27 @@
         <v>27</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.25</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="H21" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3E8</v>
       </c>
       <c r="I21" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J21" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="1">
         <v>-41</v>
       </c>
@@ -1366,27 +1434,30 @@
         <v>28</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1067</v>
       </c>
       <c r="H22" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>42B</v>
       </c>
       <c r="I22" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333325754</v>
       </c>
       <c r="J22" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3.1240237425797334E-4</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="1">
         <v>-40</v>
       </c>
@@ -1405,27 +1476,30 @@
         <v>29</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.4166666666666665</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1133</v>
       </c>
       <c r="H23" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>46D</v>
       </c>
       <c r="I23" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333325754</v>
       </c>
       <c r="J23" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-2.9420417769925641E-4</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="1">
         <v>-39</v>
       </c>
@@ -1444,27 +1518,27 @@
         <v>30</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1200</v>
       </c>
       <c r="H24" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4B0</v>
       </c>
       <c r="I24" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J24" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="1">
         <v>-38</v>
       </c>
@@ -1483,27 +1557,30 @@
         <v>31</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.5833333333333333</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1267</v>
       </c>
       <c r="H25" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4F3</v>
       </c>
       <c r="I25" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
       <c r="J25" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.6308866087883579E-4</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="1">
         <v>-37</v>
       </c>
@@ -1522,27 +1599,27 @@
         <v>32</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1333</v>
       </c>
       <c r="H26" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>535</v>
       </c>
       <c r="I26" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333325754</v>
       </c>
       <c r="J26" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-2.5006251562885039E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:11">
       <c r="A27" s="1">
         <v>-36</v>
       </c>
@@ -1561,27 +1638,30 @@
         <v>33</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.75</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1400</v>
       </c>
       <c r="H27" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>578</v>
       </c>
       <c r="I27" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J27" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="1">
         <v>-35</v>
       </c>
@@ -1600,27 +1680,27 @@
         <v>34</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.8333333333333333</v>
       </c>
       <c r="G28" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1467</v>
       </c>
       <c r="H28" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5BB</v>
       </c>
       <c r="I28" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
       <c r="J28" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.2722108611689497E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:11">
       <c r="A29" s="1">
         <v>-34</v>
       </c>
@@ -1639,27 +1719,30 @@
         <v>35</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.9166666666666665</v>
       </c>
       <c r="G29" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1533</v>
       </c>
       <c r="H29" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5FD</v>
       </c>
       <c r="I29" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333325754</v>
       </c>
       <c r="J29" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-2.1743857360290771E-4</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="1">
         <v>-33</v>
       </c>
@@ -1678,27 +1761,30 @@
         <v>36</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G30" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1600</v>
       </c>
       <c r="H30" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>640</v>
       </c>
       <c r="I30" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J30" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="1">
         <v>-32</v>
       </c>
@@ -1717,27 +1803,27 @@
         <v>37</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.083333333333333</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1667</v>
       </c>
       <c r="H31" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>683</v>
       </c>
       <c r="I31" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
       <c r="J31" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1.9996000799849125E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:11">
       <c r="A32" s="1">
         <v>-31</v>
       </c>
@@ -1756,27 +1842,30 @@
         <v>38</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.1666666666666665</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1733</v>
       </c>
       <c r="H32" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6C5</v>
       </c>
       <c r="I32" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333325754</v>
       </c>
       <c r="J32" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1.9234468166950811E-4</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="K32" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="1">
         <v>-30</v>
       </c>
@@ -1795,27 +1884,27 @@
         <v>39</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.25</v>
       </c>
       <c r="G33" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1800</v>
       </c>
       <c r="H33" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>708</v>
       </c>
       <c r="I33" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J33" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="1">
         <v>-29</v>
       </c>
@@ -1834,27 +1923,30 @@
         <v>40</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.333333333333333</v>
       </c>
       <c r="G34" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1867</v>
       </c>
       <c r="H34" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>74B</v>
       </c>
       <c r="I34" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
       <c r="J34" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1.7853954650963306E-4</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="K34" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="1">
         <v>-28</v>
       </c>
@@ -1873,27 +1965,30 @@
         <v>41</v>
       </c>
       <c r="F35" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.4166666666666665</v>
       </c>
       <c r="G35" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1933</v>
       </c>
       <c r="H35" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>78D</v>
       </c>
       <c r="I35" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333303017</v>
       </c>
       <c r="J35" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1.7244352474548897E-4</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="K35" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="1">
         <v>-27</v>
       </c>
@@ -1912,27 +2007,27 @@
         <v>42</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="H36" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>7D0</v>
       </c>
       <c r="I36" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J36" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" s="1">
         <v>-26</v>
       </c>
@@ -1951,27 +2046,30 @@
         <v>43</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.583333333333333</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2067</v>
       </c>
       <c r="H37" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>813</v>
       </c>
       <c r="I37" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
       <c r="J37" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1.6126431220778176E-4</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="K37" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="1">
         <v>-25</v>
       </c>
@@ -1990,27 +2088,27 @@
         <v>44</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="G38" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2133</v>
       </c>
       <c r="H38" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>855</v>
       </c>
       <c r="I38" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333348492</v>
       </c>
       <c r="J38" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1.5627441787786447E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:11">
       <c r="A39" s="1">
         <v>-24</v>
       </c>
@@ -2029,27 +2127,30 @@
         <v>45</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.75</v>
       </c>
       <c r="G39" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2200</v>
       </c>
       <c r="H39" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>898</v>
       </c>
       <c r="I39" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J39" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" s="1">
         <v>-23</v>
       </c>
@@ -2068,27 +2169,27 @@
         <v>46</v>
       </c>
       <c r="F40" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.833333333333333</v>
       </c>
       <c r="G40" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2267</v>
       </c>
       <c r="H40" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8DB</v>
       </c>
       <c r="I40" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
       <c r="J40" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1.4703720041177104E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:11">
       <c r="A41" s="1">
         <v>-22</v>
       </c>
@@ -2107,27 +2208,30 @@
         <v>47</v>
       </c>
       <c r="F41" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.9166666666666665</v>
       </c>
       <c r="G41" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2333</v>
       </c>
       <c r="H41" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>91D</v>
       </c>
       <c r="I41" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333303017</v>
       </c>
       <c r="J41" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1.4287755393614668E-4</v>
       </c>
-    </row>
-    <row r="42" spans="1:10">
+      <c r="K41" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" s="1">
         <v>-21</v>
       </c>
@@ -2146,27 +2250,30 @@
         <v>48</v>
       </c>
       <c r="F42" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="G42" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2400</v>
       </c>
       <c r="H42" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>960</v>
       </c>
       <c r="I42" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J42" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" s="1">
         <v>-20</v>
       </c>
@@ -2185,27 +2292,27 @@
         <v>49</v>
       </c>
       <c r="F43" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.083333333333333</v>
       </c>
       <c r="G43" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2467</v>
       </c>
       <c r="H43" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>9A3</v>
       </c>
       <c r="I43" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
       <c r="J43" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1.3511687609788606E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:11">
       <c r="A44" s="1">
         <v>-19</v>
       </c>
@@ -2224,27 +2331,30 @@
         <v>50</v>
       </c>
       <c r="F44" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.1666666666666665</v>
       </c>
       <c r="G44" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2533</v>
       </c>
       <c r="H44" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>9E5</v>
       </c>
       <c r="I44" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333303017</v>
       </c>
       <c r="J44" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1.315962626660206E-4</v>
       </c>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="K44" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" s="1">
         <v>-18</v>
       </c>
@@ -2263,27 +2373,27 @@
         <v>51</v>
       </c>
       <c r="F45" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.25</v>
       </c>
       <c r="G45" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2600</v>
       </c>
       <c r="H45" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>A28</v>
       </c>
       <c r="I45" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J45" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="1">
         <v>-17</v>
       </c>
@@ -2302,27 +2412,30 @@
         <v>52</v>
       </c>
       <c r="F46" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.333333333333333</v>
       </c>
       <c r="G46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2667</v>
       </c>
       <c r="H46" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>A6B</v>
       </c>
       <c r="I46" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
       <c r="J46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1.2498437695293772E-4</v>
       </c>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="K46" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" s="1">
         <v>-16</v>
       </c>
@@ -2341,27 +2454,30 @@
         <v>53</v>
       </c>
       <c r="F47" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.4166666666666665</v>
       </c>
       <c r="G47" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2733</v>
       </c>
       <c r="H47" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AAD</v>
       </c>
       <c r="I47" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333348492</v>
       </c>
       <c r="J47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1.2196609342608302E-4</v>
       </c>
-    </row>
-    <row r="48" spans="1:10">
+      <c r="K47" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" s="1">
         <v>-15</v>
       </c>
@@ -2380,27 +2496,27 @@
         <v>54</v>
       </c>
       <c r="F48" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.5</v>
       </c>
       <c r="G48" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2800</v>
       </c>
       <c r="H48" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AF0</v>
       </c>
       <c r="I48" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J48" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" s="1">
         <v>-14</v>
       </c>
@@ -2419,27 +2535,30 @@
         <v>55</v>
       </c>
       <c r="F49" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.583333333333333</v>
       </c>
       <c r="G49" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2867</v>
       </c>
       <c r="H49" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>B33</v>
       </c>
       <c r="I49" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333393966</v>
       </c>
       <c r="J49" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1.1626555051759318E-4</v>
       </c>
-    </row>
-    <row r="50" spans="1:10">
+      <c r="K49" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" s="1">
         <v>-13</v>
       </c>
@@ -2458,27 +2577,27 @@
         <v>56</v>
       </c>
       <c r="F50" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.6666666666666665</v>
       </c>
       <c r="G50" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2933</v>
       </c>
       <c r="H50" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>B75</v>
       </c>
       <c r="I50" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333303017</v>
       </c>
       <c r="J50" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1.1364927832697926E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:11">
       <c r="A51" s="1">
         <v>-12</v>
       </c>
@@ -2497,27 +2616,30 @@
         <v>57</v>
       </c>
       <c r="F51" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.75</v>
       </c>
       <c r="G51" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3000</v>
       </c>
       <c r="H51" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>BB8</v>
       </c>
       <c r="I51" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J51" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" s="1">
         <v>-11</v>
       </c>
@@ -2536,27 +2658,27 @@
         <v>58</v>
       </c>
       <c r="F52" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.833333333333333</v>
       </c>
       <c r="G52" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3067</v>
       </c>
       <c r="H52" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>BFB</v>
       </c>
       <c r="I52" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
       <c r="J52" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1.0868383871323278E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:11">
       <c r="A53" s="1">
         <v>-10</v>
       </c>
@@ -2575,27 +2697,30 @@
         <v>59</v>
       </c>
       <c r="F53" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.9166666666666665</v>
       </c>
       <c r="G53" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3133</v>
       </c>
       <c r="H53" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>C3D</v>
       </c>
       <c r="I53" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333348492</v>
       </c>
       <c r="J53" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1.0639429726571494E-4</v>
       </c>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="K53" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" s="1">
         <v>-9</v>
       </c>
@@ -2614,27 +2739,30 @@
         <v>60</v>
       </c>
       <c r="F54" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G54" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3200</v>
       </c>
       <c r="H54" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>C80</v>
       </c>
       <c r="I54" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J54" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="1">
         <v>-8</v>
       </c>
@@ -2653,27 +2781,27 @@
         <v>61</v>
       </c>
       <c r="F55" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4.083333333333333</v>
       </c>
       <c r="G55" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3267</v>
       </c>
       <c r="H55" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>CC3</v>
       </c>
       <c r="I55" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
       <c r="J55" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1.0203040506075449E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:11">
       <c r="A56" s="1">
         <v>-7</v>
       </c>
@@ -2692,27 +2820,30 @@
         <v>62</v>
       </c>
       <c r="F56" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666661</v>
       </c>
       <c r="G56" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3333</v>
       </c>
       <c r="H56" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>D05</v>
       </c>
       <c r="I56" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.33333333333303017</v>
       </c>
       <c r="J56" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1.0001000100000905E-4</v>
       </c>
-    </row>
-    <row r="57" spans="1:10">
+      <c r="K56" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="1">
         <v>-6</v>
       </c>
@@ -2731,27 +2862,27 @@
         <v>63</v>
       </c>
       <c r="F57" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4.25</v>
       </c>
       <c r="G57" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3400</v>
       </c>
       <c r="H57" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>D48</v>
       </c>
       <c r="I57" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J57" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" s="1">
         <v>-5</v>
       </c>
@@ -2770,27 +2901,30 @@
         <v>64</v>
       </c>
       <c r="F58" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4.333333333333333</v>
       </c>
       <c r="G58" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3467</v>
       </c>
       <c r="H58" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>D8B</v>
       </c>
       <c r="I58" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
       <c r="J58" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>9.6144601480670588E-5</v>
       </c>
-    </row>
-    <row r="59" spans="1:10">
+      <c r="K58" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" s="1">
         <v>-4</v>
       </c>
@@ -2809,27 +2943,30 @@
         <v>65</v>
       </c>
       <c r="F59" s="3">
-        <f t="shared" si="2"/>
-        <v>-1.75</v>
+        <f t="shared" si="6"/>
+        <v>4.4166666666666661</v>
       </c>
       <c r="G59" s="3">
-        <f t="shared" si="3"/>
-        <v>-1400</v>
+        <f t="shared" si="2"/>
+        <v>3533</v>
       </c>
       <c r="H59" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>FFFFFFFA88</v>
+        <f t="shared" si="4"/>
+        <v>DCD</v>
       </c>
       <c r="I59" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>-0.33333333333257542</v>
       </c>
       <c r="J59" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>-9.4348523445393555E-5</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" s="1">
         <v>-3</v>
       </c>
@@ -2848,27 +2985,27 @@
         <v>66</v>
       </c>
       <c r="F60" s="3">
-        <f t="shared" si="2"/>
-        <v>-1.75</v>
+        <f t="shared" si="6"/>
+        <v>4.5</v>
       </c>
       <c r="G60" s="3">
-        <f t="shared" si="3"/>
-        <v>-1400</v>
+        <f t="shared" si="2"/>
+        <v>3600</v>
       </c>
       <c r="H60" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>FFFFFFFA88</v>
+        <f t="shared" si="4"/>
+        <v>E10</v>
       </c>
       <c r="I60" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J60" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" s="1">
         <v>-2</v>
       </c>
@@ -2887,27 +3024,30 @@
         <v>67</v>
       </c>
       <c r="F61" s="3">
-        <f t="shared" si="2"/>
-        <v>-1.75</v>
+        <f t="shared" si="6"/>
+        <v>4.583333333333333</v>
       </c>
       <c r="G61" s="3">
-        <f t="shared" si="3"/>
-        <v>-1400</v>
+        <f t="shared" si="2"/>
+        <v>3667</v>
       </c>
       <c r="H61" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>FFFFFFFA88</v>
+        <f t="shared" si="4"/>
+        <v>E53</v>
       </c>
       <c r="I61" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.33333333333348492</v>
       </c>
       <c r="J61" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>9.0900827197568838E-5</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62" s="1">
         <v>-1</v>
       </c>
@@ -2926,27 +3066,27 @@
         <v>68</v>
       </c>
       <c r="F62" s="3">
-        <f t="shared" si="2"/>
-        <v>-1.75</v>
+        <f t="shared" si="6"/>
+        <v>4.6666666666666661</v>
       </c>
       <c r="G62" s="3">
-        <f t="shared" si="3"/>
-        <v>-1400</v>
+        <f t="shared" si="2"/>
+        <v>3733</v>
       </c>
       <c r="H62" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>FFFFFFFA88</v>
+        <f t="shared" si="4"/>
+        <v>E95</v>
       </c>
       <c r="I62" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>-0.33333333333303017</v>
       </c>
       <c r="J62" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>-8.9293686936252388E-5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63" s="1">
         <v>0</v>
       </c>
@@ -2965,27 +3105,30 @@
         <v>69</v>
       </c>
       <c r="F63" s="3">
-        <f t="shared" si="2"/>
-        <v>-1.75</v>
+        <f t="shared" si="6"/>
+        <v>4.75</v>
       </c>
       <c r="G63" s="3">
-        <f t="shared" si="3"/>
-        <v>-1400</v>
+        <f t="shared" si="2"/>
+        <v>3800</v>
       </c>
       <c r="H63" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>FFFFFFFA88</v>
+        <f t="shared" si="4"/>
+        <v>ED8</v>
       </c>
       <c r="I63" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J63" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64" s="1">
         <v>1</v>
       </c>
@@ -3004,27 +3147,27 @@
         <v>70</v>
       </c>
       <c r="F64" s="3">
-        <f t="shared" si="2"/>
-        <v>-1.75</v>
+        <f t="shared" si="6"/>
+        <v>4.833333333333333</v>
       </c>
       <c r="G64" s="3">
-        <f t="shared" si="3"/>
-        <v>-1400</v>
+        <f t="shared" si="2"/>
+        <v>3867</v>
       </c>
       <c r="H64" s="3" t="str">
         <f>DEC2HEX(G64,3)</f>
-        <v>FFFFFFFA88</v>
+        <v>F1B</v>
       </c>
       <c r="I64" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.33333333333393966</v>
       </c>
       <c r="J64" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>8.6199465563470309E-5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" s="1">
         <v>2</v>
       </c>
@@ -3043,27 +3186,30 @@
         <v>71</v>
       </c>
       <c r="F65" s="3">
-        <f t="shared" si="2"/>
-        <v>-1.75</v>
+        <f t="shared" si="6"/>
+        <v>4.9166666666666661</v>
       </c>
       <c r="G65" s="3">
-        <f t="shared" si="3"/>
-        <v>-1400</v>
+        <f t="shared" si="2"/>
+        <v>3933</v>
       </c>
       <c r="H65" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>FFFFFFFA88</v>
+        <f t="shared" si="4"/>
+        <v>F5D</v>
       </c>
       <c r="I65" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>-0.33333333333257542</v>
       </c>
       <c r="J65" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>-8.4752945164651776E-5</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" s="1">
         <v>3</v>
       </c>
@@ -3082,27 +3228,30 @@
         <v>72</v>
       </c>
       <c r="F66" s="3">
-        <f t="shared" si="2"/>
-        <v>-1.75</v>
+        <f t="shared" si="6"/>
+        <v>5</v>
       </c>
       <c r="G66" s="3">
-        <f t="shared" si="3"/>
-        <v>-1400</v>
+        <f t="shared" si="2"/>
+        <v>4000</v>
       </c>
       <c r="H66" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>FFFFFFFA88</v>
+        <f t="shared" si="4"/>
+        <v>FA0</v>
       </c>
       <c r="I66" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J66" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67" s="1">
         <v>4</v>
       </c>
@@ -3121,28 +3270,29 @@
         <v>73</v>
       </c>
       <c r="F67" s="3">
-        <f t="shared" si="2"/>
-        <v>-1.75</v>
+        <f t="shared" si="6"/>
+        <v>5.083333333333333</v>
       </c>
       <c r="G67" s="3">
-        <f t="shared" si="3"/>
-        <v>-1400</v>
+        <f t="shared" si="2"/>
+        <v>4067</v>
       </c>
       <c r="H67" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>FFFFFFFA88</v>
+        <f t="shared" si="4"/>
+        <v>FE3</v>
       </c>
       <c r="I67" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.33333333333348492</v>
       </c>
       <c r="J67" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>8.196049504142732E-5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Basic wavetable sweeps working
</commit_message>
<xml_diff>
--- a/documentation/b/cv-notes.xlsx
+++ b/documentation/b/cv-notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1380" yWindow="3920" windowWidth="25600" windowHeight="28280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3292,7 +3292,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
major refactor of Key (and saved about 1kB)
</commit_message>
<xml_diff>
--- a/documentation/b/cv-notes.xlsx
+++ b/documentation/b/cv-notes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="3920" windowWidth="25600" windowHeight="28280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="101">
   <si>
     <t>Note: The data my calculations are based on are based on a spreadsheet from http://obsoletetechnology.wordpress.com/projects/midi-cvgate-converter/</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>mV</t>
   </si>
 </sst>
 </file>
@@ -375,8 +378,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -393,9 +404,17 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -725,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K67"/>
+  <dimension ref="A2:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -736,12 +755,12 @@
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="2" customFormat="1">
+    <row r="5" spans="1:13" s="2" customFormat="1">
       <c r="A5" s="2" t="s">
         <v>86</v>
       </c>
@@ -755,19 +774,22 @@
         <v>88</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:13">
       <c r="A6" s="1">
         <v>-57</v>
       </c>
@@ -790,23 +812,27 @@
         <v>0</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" ref="G6:G67" si="2">ROUND((F6/1.25)*1000,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="3" t="str">
-        <f>DEC2HEX(G6,3)</f>
+        <f>ROUND(F6*1000, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" ref="H6:H67" si="2">ROUND((F6/1.25)*1000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="3" t="str">
+        <f>DEC2HEX(H6,3)</f>
         <v>000</v>
       </c>
-      <c r="I6" s="3">
-        <f t="shared" ref="I6:I67" si="3">G6-(F6/1.25)*1000</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="1" t="s">
+      <c r="J6" s="3">
+        <f t="shared" ref="J6:J67" si="3">H6-(F6/1.25)*1000</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:13">
       <c r="A7" s="1">
         <v>-56</v>
       </c>
@@ -829,23 +855,27 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="G7" s="3">
+        <f t="shared" ref="G7:G18" si="4">ROUND(F7*1000, 0)</f>
+        <v>83</v>
+      </c>
+      <c r="H7" s="3">
         <f t="shared" si="2"/>
         <v>67</v>
       </c>
-      <c r="H7" s="3" t="str">
-        <f>DEC2HEX(G7,3)</f>
+      <c r="I7" s="3" t="str">
+        <f>DEC2HEX(H7,3)</f>
         <v>043</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <f t="shared" si="3"/>
         <v>0.3333333333333286</v>
       </c>
-      <c r="J7" s="5">
-        <f>I7/G7</f>
+      <c r="K7" s="5">
+        <f>J7/H7</f>
         <v>4.9751243781093824E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:13">
       <c r="A8" s="1">
         <v>-55</v>
       </c>
@@ -868,26 +898,30 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="G8" s="3">
+        <f t="shared" si="4"/>
+        <v>167</v>
+      </c>
+      <c r="H8" s="3">
         <f t="shared" si="2"/>
         <v>133</v>
       </c>
-      <c r="H8" s="3" t="str">
-        <f t="shared" ref="H8:H67" si="4">DEC2HEX(G8,3)</f>
+      <c r="I8" s="3" t="str">
+        <f t="shared" ref="I8:I67" si="5">DEC2HEX(H8,3)</f>
         <v>085</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333334281</v>
       </c>
-      <c r="J8" s="5">
-        <f t="shared" ref="J8:J67" si="5">I8/G8</f>
+      <c r="K8" s="5">
+        <f t="shared" ref="K8:K67" si="6">J8/H8</f>
         <v>-2.5062656641604724E-3</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:13">
       <c r="A9" s="1">
         <v>-54</v>
       </c>
@@ -906,27 +940,34 @@
         <v>15</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" ref="F9:F67" si="6">(1/12)*(E9-12)</f>
+        <f t="shared" ref="F9:F67" si="7">(1/12)*(E9-12)</f>
         <v>0.25</v>
       </c>
       <c r="G9" s="3">
+        <f t="shared" si="4"/>
+        <v>250</v>
+      </c>
+      <c r="H9" s="3">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-      <c r="H9" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I9" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>0C8</v>
       </c>
-      <c r="I9" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="J9" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>134940</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1">
         <v>-53</v>
       </c>
@@ -945,30 +986,34 @@
         <v>16</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G10" s="3">
+        <f t="shared" si="4"/>
+        <v>333</v>
+      </c>
+      <c r="H10" s="3">
         <f t="shared" si="2"/>
         <v>267</v>
       </c>
-      <c r="H10" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I10" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>10B</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333331439</v>
       </c>
-      <c r="J10" s="5">
-        <f t="shared" si="5"/>
+      <c r="K10" s="5">
+        <f t="shared" si="6"/>
         <v>1.2484394506865708E-3</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:13">
       <c r="A11" s="1">
         <v>-52</v>
       </c>
@@ -987,30 +1032,34 @@
         <v>17</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.41666666666666663</v>
       </c>
       <c r="G11" s="3">
+        <f t="shared" si="4"/>
+        <v>417</v>
+      </c>
+      <c r="H11" s="3">
         <f t="shared" si="2"/>
         <v>333</v>
       </c>
-      <c r="H11" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I11" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>14D</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333331439</v>
       </c>
-      <c r="J11" s="5">
-        <f t="shared" si="5"/>
+      <c r="K11" s="5">
+        <f t="shared" si="6"/>
         <v>-1.0010010010009442E-3</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:13">
       <c r="A12" s="1">
         <v>-51</v>
       </c>
@@ -1029,27 +1078,31 @@
         <v>18</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
       <c r="G12" s="3">
+        <f t="shared" si="4"/>
+        <v>500</v>
+      </c>
+      <c r="H12" s="3">
         <f t="shared" si="2"/>
         <v>400</v>
       </c>
-      <c r="H12" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I12" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>190</v>
       </c>
-      <c r="I12" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="J12" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1">
         <v>-50</v>
       </c>
@@ -1068,30 +1121,34 @@
         <v>19</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.58333333333333326</v>
       </c>
       <c r="G13" s="3">
+        <f t="shared" si="4"/>
+        <v>583</v>
+      </c>
+      <c r="H13" s="3">
         <f t="shared" si="2"/>
         <v>467</v>
       </c>
-      <c r="H13" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I13" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>1D3</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333337123</v>
       </c>
-      <c r="J13" s="5">
-        <f t="shared" si="5"/>
+      <c r="K13" s="5">
+        <f t="shared" si="6"/>
         <v>7.1377587437552721E-4</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:13">
       <c r="A14" s="1">
         <v>-49</v>
       </c>
@@ -1110,27 +1167,31 @@
         <v>20</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="G14" s="3">
+        <f t="shared" si="4"/>
+        <v>667</v>
+      </c>
+      <c r="H14" s="3">
         <f t="shared" si="2"/>
         <v>533</v>
       </c>
-      <c r="H14" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I14" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>215</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333337123</v>
       </c>
-      <c r="J14" s="5">
-        <f t="shared" si="5"/>
+      <c r="K14" s="5">
+        <f t="shared" si="6"/>
         <v>-6.2539086929337944E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:13">
       <c r="A15" s="1">
         <v>-48</v>
       </c>
@@ -1149,30 +1210,34 @@
         <v>21</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.75</v>
       </c>
       <c r="G15" s="3">
+        <f t="shared" si="4"/>
+        <v>750</v>
+      </c>
+      <c r="H15" s="3">
         <f t="shared" si="2"/>
         <v>600</v>
       </c>
-      <c r="H15" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I15" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>258</v>
       </c>
-      <c r="I15" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="1" t="s">
+      <c r="J15" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:13">
       <c r="A16" s="1">
         <v>-47</v>
       </c>
@@ -1191,27 +1256,31 @@
         <v>22</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.83333333333333326</v>
       </c>
       <c r="G16" s="3">
+        <f t="shared" si="4"/>
+        <v>833</v>
+      </c>
+      <c r="H16" s="3">
         <f t="shared" si="2"/>
         <v>667</v>
       </c>
-      <c r="H16" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I16" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>29B</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333337123</v>
       </c>
-      <c r="J16" s="5">
-        <f t="shared" si="5"/>
+      <c r="K16" s="5">
+        <f t="shared" si="6"/>
         <v>4.9975012493758803E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>-46</v>
       </c>
@@ -1230,30 +1299,34 @@
         <v>23</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.91666666666666663</v>
       </c>
       <c r="G17" s="3">
+        <f t="shared" si="4"/>
+        <v>917</v>
+      </c>
+      <c r="H17" s="3">
         <f t="shared" si="2"/>
         <v>733</v>
       </c>
-      <c r="H17" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I17" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>2DD</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333325754</v>
       </c>
-      <c r="J17" s="5">
-        <f t="shared" si="5"/>
+      <c r="K17" s="5">
+        <f t="shared" si="6"/>
         <v>-4.5475216007265695E-4</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>-45</v>
       </c>
@@ -1272,30 +1345,34 @@
         <v>24</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G18" s="3">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="H18" s="3">
         <f t="shared" si="2"/>
         <v>800</v>
       </c>
-      <c r="H18" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I18" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>320</v>
       </c>
-      <c r="I18" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K18" s="1" t="s">
+      <c r="J18" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>-44</v>
       </c>
@@ -1314,27 +1391,28 @@
         <v>25</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0833333333333333</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="3"/>
+      <c r="H19" s="3">
         <f t="shared" si="2"/>
         <v>867</v>
       </c>
-      <c r="H19" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I19" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>363</v>
       </c>
-      <c r="I19" s="3">
+      <c r="J19" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333337123</v>
       </c>
-      <c r="J19" s="5">
-        <f t="shared" si="5"/>
+      <c r="K19" s="5">
+        <f t="shared" si="6"/>
         <v>3.8446751249523786E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>-43</v>
       </c>
@@ -1353,30 +1431,31 @@
         <v>26</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1666666666666665</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="3"/>
+      <c r="H20" s="3">
         <f t="shared" si="2"/>
         <v>933</v>
       </c>
-      <c r="H20" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I20" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>3A5</v>
       </c>
-      <c r="I20" s="3">
+      <c r="J20" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333325754</v>
       </c>
-      <c r="J20" s="5">
-        <f t="shared" si="5"/>
+      <c r="K20" s="5">
+        <f t="shared" si="6"/>
         <v>-3.5727045373339501E-4</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>-42</v>
       </c>
@@ -1395,27 +1474,28 @@
         <v>27</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.25</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="3"/>
+      <c r="H21" s="3">
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
-      <c r="H21" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I21" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>3E8</v>
       </c>
-      <c r="I21" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="J21" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>-41</v>
       </c>
@@ -1434,30 +1514,31 @@
         <v>28</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="3"/>
+      <c r="H22" s="3">
         <f t="shared" si="2"/>
         <v>1067</v>
       </c>
-      <c r="H22" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I22" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>42B</v>
       </c>
-      <c r="I22" s="3">
+      <c r="J22" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333325754</v>
       </c>
-      <c r="J22" s="5">
-        <f t="shared" si="5"/>
+      <c r="K22" s="5">
+        <f t="shared" si="6"/>
         <v>3.1240237425797334E-4</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:12">
       <c r="A23" s="1">
         <v>-40</v>
       </c>
@@ -1476,30 +1557,31 @@
         <v>29</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.4166666666666665</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="3"/>
+      <c r="H23" s="3">
         <f t="shared" si="2"/>
         <v>1133</v>
       </c>
-      <c r="H23" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I23" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>46D</v>
       </c>
-      <c r="I23" s="3">
+      <c r="J23" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333325754</v>
       </c>
-      <c r="J23" s="5">
-        <f t="shared" si="5"/>
+      <c r="K23" s="5">
+        <f t="shared" si="6"/>
         <v>-2.9420417769925641E-4</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>-39</v>
       </c>
@@ -1518,27 +1600,28 @@
         <v>30</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.5</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="3"/>
+      <c r="H24" s="3">
         <f t="shared" si="2"/>
         <v>1200</v>
       </c>
-      <c r="H24" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I24" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>4B0</v>
       </c>
-      <c r="I24" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="J24" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>-38</v>
       </c>
@@ -1557,30 +1640,31 @@
         <v>31</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.5833333333333333</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="3"/>
+      <c r="H25" s="3">
         <f t="shared" si="2"/>
         <v>1267</v>
       </c>
-      <c r="H25" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I25" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>4F3</v>
       </c>
-      <c r="I25" s="3">
+      <c r="J25" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
-      <c r="J25" s="5">
-        <f t="shared" si="5"/>
+      <c r="K25" s="5">
+        <f t="shared" si="6"/>
         <v>2.6308866087883579E-4</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:12">
       <c r="A26" s="1">
         <v>-37</v>
       </c>
@@ -1599,27 +1683,28 @@
         <v>32</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6666666666666665</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="3"/>
+      <c r="H26" s="3">
         <f t="shared" si="2"/>
         <v>1333</v>
       </c>
-      <c r="H26" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I26" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>535</v>
       </c>
-      <c r="I26" s="3">
+      <c r="J26" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333325754</v>
       </c>
-      <c r="J26" s="5">
-        <f t="shared" si="5"/>
+      <c r="K26" s="5">
+        <f t="shared" si="6"/>
         <v>-2.5006251562885039E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:12">
       <c r="A27" s="1">
         <v>-36</v>
       </c>
@@ -1638,30 +1723,31 @@
         <v>33</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.75</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="3"/>
+      <c r="H27" s="3">
         <f t="shared" si="2"/>
         <v>1400</v>
       </c>
-      <c r="H27" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I27" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>578</v>
       </c>
-      <c r="I27" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K27" s="1" t="s">
+      <c r="J27" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:12">
       <c r="A28" s="1">
         <v>-35</v>
       </c>
@@ -1680,27 +1766,28 @@
         <v>34</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.8333333333333333</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="3"/>
+      <c r="H28" s="3">
         <f t="shared" si="2"/>
         <v>1467</v>
       </c>
-      <c r="H28" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I28" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>5BB</v>
       </c>
-      <c r="I28" s="3">
+      <c r="J28" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
-      <c r="J28" s="5">
-        <f t="shared" si="5"/>
+      <c r="K28" s="5">
+        <f t="shared" si="6"/>
         <v>2.2722108611689497E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:12">
       <c r="A29" s="1">
         <v>-34</v>
       </c>
@@ -1719,30 +1806,31 @@
         <v>35</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.9166666666666665</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="3"/>
+      <c r="H29" s="3">
         <f t="shared" si="2"/>
         <v>1533</v>
       </c>
-      <c r="H29" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I29" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>5FD</v>
       </c>
-      <c r="I29" s="3">
+      <c r="J29" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333325754</v>
       </c>
-      <c r="J29" s="5">
-        <f t="shared" si="5"/>
+      <c r="K29" s="5">
+        <f t="shared" si="6"/>
         <v>-2.1743857360290771E-4</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:12">
       <c r="A30" s="1">
         <v>-33</v>
       </c>
@@ -1761,30 +1849,31 @@
         <v>36</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="3"/>
+      <c r="H30" s="3">
         <f t="shared" si="2"/>
         <v>1600</v>
       </c>
-      <c r="H30" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I30" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>640</v>
       </c>
-      <c r="I30" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J30" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K30" s="1" t="s">
+      <c r="J30" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:12">
       <c r="A31" s="1">
         <v>-32</v>
       </c>
@@ -1803,27 +1892,28 @@
         <v>37</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.083333333333333</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="3"/>
+      <c r="H31" s="3">
         <f t="shared" si="2"/>
         <v>1667</v>
       </c>
-      <c r="H31" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I31" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>683</v>
       </c>
-      <c r="I31" s="3">
+      <c r="J31" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
-      <c r="J31" s="5">
-        <f t="shared" si="5"/>
+      <c r="K31" s="5">
+        <f t="shared" si="6"/>
         <v>1.9996000799849125E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:12">
       <c r="A32" s="1">
         <v>-31</v>
       </c>
@@ -1842,30 +1932,31 @@
         <v>38</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1666666666666665</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32" s="3"/>
+      <c r="H32" s="3">
         <f t="shared" si="2"/>
         <v>1733</v>
       </c>
-      <c r="H32" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I32" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>6C5</v>
       </c>
-      <c r="I32" s="3">
+      <c r="J32" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333325754</v>
       </c>
-      <c r="J32" s="5">
-        <f t="shared" si="5"/>
+      <c r="K32" s="5">
+        <f t="shared" si="6"/>
         <v>-1.9234468166950811E-4</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:12">
       <c r="A33" s="1">
         <v>-30</v>
       </c>
@@ -1884,27 +1975,28 @@
         <v>39</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.25</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G33" s="3"/>
+      <c r="H33" s="3">
         <f t="shared" si="2"/>
         <v>1800</v>
       </c>
-      <c r="H33" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I33" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>708</v>
       </c>
-      <c r="I33" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="J33" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="1">
         <v>-29</v>
       </c>
@@ -1923,30 +2015,31 @@
         <v>40</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.333333333333333</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="3"/>
+      <c r="H34" s="3">
         <f t="shared" si="2"/>
         <v>1867</v>
       </c>
-      <c r="H34" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I34" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>74B</v>
       </c>
-      <c r="I34" s="3">
+      <c r="J34" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
-      <c r="J34" s="5">
-        <f t="shared" si="5"/>
+      <c r="K34" s="5">
+        <f t="shared" si="6"/>
         <v>1.7853954650963306E-4</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:12">
       <c r="A35" s="1">
         <v>-28</v>
       </c>
@@ -1965,30 +2058,31 @@
         <v>41</v>
       </c>
       <c r="F35" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4166666666666665</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35" s="3"/>
+      <c r="H35" s="3">
         <f t="shared" si="2"/>
         <v>1933</v>
       </c>
-      <c r="H35" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I35" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>78D</v>
       </c>
-      <c r="I35" s="3">
+      <c r="J35" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333303017</v>
       </c>
-      <c r="J35" s="5">
-        <f t="shared" si="5"/>
+      <c r="K35" s="5">
+        <f t="shared" si="6"/>
         <v>-1.7244352474548897E-4</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:12">
       <c r="A36" s="1">
         <v>-27</v>
       </c>
@@ -2007,27 +2101,28 @@
         <v>42</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36" s="3"/>
+      <c r="H36" s="3">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
-      <c r="H36" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I36" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>7D0</v>
       </c>
-      <c r="I36" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J36" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="J36" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K36" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="1">
         <v>-26</v>
       </c>
@@ -2046,30 +2141,31 @@
         <v>43</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.583333333333333</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37" s="3"/>
+      <c r="H37" s="3">
         <f t="shared" si="2"/>
         <v>2067</v>
       </c>
-      <c r="H37" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I37" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>813</v>
       </c>
-      <c r="I37" s="3">
+      <c r="J37" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
-      <c r="J37" s="5">
-        <f t="shared" si="5"/>
+      <c r="K37" s="5">
+        <f t="shared" si="6"/>
         <v>1.6126431220778176E-4</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:12">
       <c r="A38" s="1">
         <v>-25</v>
       </c>
@@ -2088,27 +2184,28 @@
         <v>44</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38" s="3"/>
+      <c r="H38" s="3">
         <f t="shared" si="2"/>
         <v>2133</v>
       </c>
-      <c r="H38" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I38" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>855</v>
       </c>
-      <c r="I38" s="3">
+      <c r="J38" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333348492</v>
       </c>
-      <c r="J38" s="5">
-        <f t="shared" si="5"/>
+      <c r="K38" s="5">
+        <f t="shared" si="6"/>
         <v>-1.5627441787786447E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:12">
       <c r="A39" s="1">
         <v>-24</v>
       </c>
@@ -2127,30 +2224,31 @@
         <v>45</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.75</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39" s="3"/>
+      <c r="H39" s="3">
         <f t="shared" si="2"/>
         <v>2200</v>
       </c>
-      <c r="H39" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I39" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>898</v>
       </c>
-      <c r="I39" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J39" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K39" s="1" t="s">
+      <c r="J39" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K39" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L39" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:12">
       <c r="A40" s="1">
         <v>-23</v>
       </c>
@@ -2169,27 +2267,28 @@
         <v>46</v>
       </c>
       <c r="F40" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.833333333333333</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G40" s="3"/>
+      <c r="H40" s="3">
         <f t="shared" si="2"/>
         <v>2267</v>
       </c>
-      <c r="H40" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I40" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>8DB</v>
       </c>
-      <c r="I40" s="3">
+      <c r="J40" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
-      <c r="J40" s="5">
-        <f t="shared" si="5"/>
+      <c r="K40" s="5">
+        <f t="shared" si="6"/>
         <v>1.4703720041177104E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:12">
       <c r="A41" s="1">
         <v>-22</v>
       </c>
@@ -2208,30 +2307,31 @@
         <v>47</v>
       </c>
       <c r="F41" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.9166666666666665</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="3"/>
+      <c r="H41" s="3">
         <f t="shared" si="2"/>
         <v>2333</v>
       </c>
-      <c r="H41" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I41" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>91D</v>
       </c>
-      <c r="I41" s="3">
+      <c r="J41" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333303017</v>
       </c>
-      <c r="J41" s="5">
-        <f t="shared" si="5"/>
+      <c r="K41" s="5">
+        <f t="shared" si="6"/>
         <v>-1.4287755393614668E-4</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="L41" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:12">
       <c r="A42" s="1">
         <v>-21</v>
       </c>
@@ -2250,30 +2350,31 @@
         <v>48</v>
       </c>
       <c r="F42" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="3"/>
+      <c r="H42" s="3">
         <f t="shared" si="2"/>
         <v>2400</v>
       </c>
-      <c r="H42" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I42" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>960</v>
       </c>
-      <c r="I42" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J42" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K42" s="1" t="s">
+      <c r="J42" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K42" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L42" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:12">
       <c r="A43" s="1">
         <v>-20</v>
       </c>
@@ -2292,27 +2393,28 @@
         <v>49</v>
       </c>
       <c r="F43" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.083333333333333</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G43" s="3"/>
+      <c r="H43" s="3">
         <f t="shared" si="2"/>
         <v>2467</v>
       </c>
-      <c r="H43" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I43" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>9A3</v>
       </c>
-      <c r="I43" s="3">
+      <c r="J43" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
-      <c r="J43" s="5">
-        <f t="shared" si="5"/>
+      <c r="K43" s="5">
+        <f t="shared" si="6"/>
         <v>1.3511687609788606E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:12">
       <c r="A44" s="1">
         <v>-19</v>
       </c>
@@ -2331,30 +2433,31 @@
         <v>50</v>
       </c>
       <c r="F44" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.1666666666666665</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G44" s="3"/>
+      <c r="H44" s="3">
         <f t="shared" si="2"/>
         <v>2533</v>
       </c>
-      <c r="H44" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I44" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>9E5</v>
       </c>
-      <c r="I44" s="3">
+      <c r="J44" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333303017</v>
       </c>
-      <c r="J44" s="5">
-        <f t="shared" si="5"/>
+      <c r="K44" s="5">
+        <f t="shared" si="6"/>
         <v>-1.315962626660206E-4</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="L44" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:12">
       <c r="A45" s="1">
         <v>-18</v>
       </c>
@@ -2373,27 +2476,28 @@
         <v>51</v>
       </c>
       <c r="F45" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.25</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G45" s="3"/>
+      <c r="H45" s="3">
         <f t="shared" si="2"/>
         <v>2600</v>
       </c>
-      <c r="H45" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I45" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>A28</v>
       </c>
-      <c r="I45" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J45" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="J45" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K45" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" s="1">
         <v>-17</v>
       </c>
@@ -2412,30 +2516,31 @@
         <v>52</v>
       </c>
       <c r="F46" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.333333333333333</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G46" s="3"/>
+      <c r="H46" s="3">
         <f t="shared" si="2"/>
         <v>2667</v>
       </c>
-      <c r="H46" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I46" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>A6B</v>
       </c>
-      <c r="I46" s="3">
+      <c r="J46" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
-      <c r="J46" s="5">
-        <f t="shared" si="5"/>
+      <c r="K46" s="5">
+        <f t="shared" si="6"/>
         <v>1.2498437695293772E-4</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="L46" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:12">
       <c r="A47" s="1">
         <v>-16</v>
       </c>
@@ -2454,30 +2559,31 @@
         <v>53</v>
       </c>
       <c r="F47" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.4166666666666665</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47" s="3"/>
+      <c r="H47" s="3">
         <f t="shared" si="2"/>
         <v>2733</v>
       </c>
-      <c r="H47" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I47" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>AAD</v>
       </c>
-      <c r="I47" s="3">
+      <c r="J47" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333348492</v>
       </c>
-      <c r="J47" s="5">
-        <f t="shared" si="5"/>
+      <c r="K47" s="5">
+        <f t="shared" si="6"/>
         <v>-1.2196609342608302E-4</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="L47" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:12">
       <c r="A48" s="1">
         <v>-15</v>
       </c>
@@ -2496,27 +2602,28 @@
         <v>54</v>
       </c>
       <c r="F48" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.5</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G48" s="3"/>
+      <c r="H48" s="3">
         <f t="shared" si="2"/>
         <v>2800</v>
       </c>
-      <c r="H48" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I48" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>AF0</v>
       </c>
-      <c r="I48" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J48" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
+      <c r="J48" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K48" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" s="1">
         <v>-14</v>
       </c>
@@ -2535,30 +2642,31 @@
         <v>55</v>
       </c>
       <c r="F49" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.583333333333333</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G49" s="3"/>
+      <c r="H49" s="3">
         <f t="shared" si="2"/>
         <v>2867</v>
       </c>
-      <c r="H49" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I49" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>B33</v>
       </c>
-      <c r="I49" s="3">
+      <c r="J49" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333393966</v>
       </c>
-      <c r="J49" s="5">
-        <f t="shared" si="5"/>
+      <c r="K49" s="5">
+        <f t="shared" si="6"/>
         <v>1.1626555051759318E-4</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="L49" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:12">
       <c r="A50" s="1">
         <v>-13</v>
       </c>
@@ -2577,27 +2685,28 @@
         <v>56</v>
       </c>
       <c r="F50" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.6666666666666665</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G50" s="3"/>
+      <c r="H50" s="3">
         <f t="shared" si="2"/>
         <v>2933</v>
       </c>
-      <c r="H50" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I50" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>B75</v>
       </c>
-      <c r="I50" s="3">
+      <c r="J50" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333303017</v>
       </c>
-      <c r="J50" s="5">
-        <f t="shared" si="5"/>
+      <c r="K50" s="5">
+        <f t="shared" si="6"/>
         <v>-1.1364927832697926E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:12">
       <c r="A51" s="1">
         <v>-12</v>
       </c>
@@ -2616,30 +2725,31 @@
         <v>57</v>
       </c>
       <c r="F51" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.75</v>
       </c>
-      <c r="G51" s="3">
+      <c r="G51" s="3"/>
+      <c r="H51" s="3">
         <f t="shared" si="2"/>
         <v>3000</v>
       </c>
-      <c r="H51" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I51" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>BB8</v>
       </c>
-      <c r="I51" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J51" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K51" s="1" t="s">
+      <c r="J51" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K51" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L51" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:12">
       <c r="A52" s="1">
         <v>-11</v>
       </c>
@@ -2658,27 +2768,28 @@
         <v>58</v>
       </c>
       <c r="F52" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.833333333333333</v>
       </c>
-      <c r="G52" s="3">
+      <c r="G52" s="3"/>
+      <c r="H52" s="3">
         <f t="shared" si="2"/>
         <v>3067</v>
       </c>
-      <c r="H52" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I52" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>BFB</v>
       </c>
-      <c r="I52" s="3">
+      <c r="J52" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
-      <c r="J52" s="5">
-        <f t="shared" si="5"/>
+      <c r="K52" s="5">
+        <f t="shared" si="6"/>
         <v>1.0868383871323278E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:12">
       <c r="A53" s="1">
         <v>-10</v>
       </c>
@@ -2697,30 +2808,31 @@
         <v>59</v>
       </c>
       <c r="F53" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.9166666666666665</v>
       </c>
-      <c r="G53" s="3">
+      <c r="G53" s="3"/>
+      <c r="H53" s="3">
         <f t="shared" si="2"/>
         <v>3133</v>
       </c>
-      <c r="H53" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I53" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>C3D</v>
       </c>
-      <c r="I53" s="3">
+      <c r="J53" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333348492</v>
       </c>
-      <c r="J53" s="5">
-        <f t="shared" si="5"/>
+      <c r="K53" s="5">
+        <f t="shared" si="6"/>
         <v>-1.0639429726571494E-4</v>
       </c>
-      <c r="K53" s="1" t="s">
+      <c r="L53" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:12">
       <c r="A54" s="1">
         <v>-9</v>
       </c>
@@ -2739,30 +2851,31 @@
         <v>60</v>
       </c>
       <c r="F54" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="G54" s="3">
+      <c r="G54" s="3"/>
+      <c r="H54" s="3">
         <f t="shared" si="2"/>
         <v>3200</v>
       </c>
-      <c r="H54" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I54" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>C80</v>
       </c>
-      <c r="I54" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J54" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K54" s="1" t="s">
+      <c r="J54" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K54" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L54" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:12">
       <c r="A55" s="1">
         <v>-8</v>
       </c>
@@ -2781,27 +2894,28 @@
         <v>61</v>
       </c>
       <c r="F55" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.083333333333333</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G55" s="3"/>
+      <c r="H55" s="3">
         <f t="shared" si="2"/>
         <v>3267</v>
       </c>
-      <c r="H55" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I55" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>CC3</v>
       </c>
-      <c r="I55" s="3">
+      <c r="J55" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
-      <c r="J55" s="5">
-        <f t="shared" si="5"/>
+      <c r="K55" s="5">
+        <f t="shared" si="6"/>
         <v>1.0203040506075449E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:12">
       <c r="A56" s="1">
         <v>-7</v>
       </c>
@@ -2820,30 +2934,31 @@
         <v>62</v>
       </c>
       <c r="F56" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.1666666666666661</v>
       </c>
-      <c r="G56" s="3">
+      <c r="G56" s="3"/>
+      <c r="H56" s="3">
         <f t="shared" si="2"/>
         <v>3333</v>
       </c>
-      <c r="H56" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I56" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>D05</v>
       </c>
-      <c r="I56" s="3">
+      <c r="J56" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333303017</v>
       </c>
-      <c r="J56" s="5">
-        <f t="shared" si="5"/>
+      <c r="K56" s="5">
+        <f t="shared" si="6"/>
         <v>-1.0001000100000905E-4</v>
       </c>
-      <c r="K56" s="1" t="s">
+      <c r="L56" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:12">
       <c r="A57" s="1">
         <v>-6</v>
       </c>
@@ -2862,27 +2977,28 @@
         <v>63</v>
       </c>
       <c r="F57" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.25</v>
       </c>
-      <c r="G57" s="3">
+      <c r="G57" s="3"/>
+      <c r="H57" s="3">
         <f t="shared" si="2"/>
         <v>3400</v>
       </c>
-      <c r="H57" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I57" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>D48</v>
       </c>
-      <c r="I57" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J57" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11">
+      <c r="J57" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K57" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" s="1">
         <v>-5</v>
       </c>
@@ -2901,30 +3017,31 @@
         <v>64</v>
       </c>
       <c r="F58" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.333333333333333</v>
       </c>
-      <c r="G58" s="3">
+      <c r="G58" s="3"/>
+      <c r="H58" s="3">
         <f t="shared" si="2"/>
         <v>3467</v>
       </c>
-      <c r="H58" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I58" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>D8B</v>
       </c>
-      <c r="I58" s="3">
+      <c r="J58" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
-      <c r="J58" s="5">
-        <f t="shared" si="5"/>
+      <c r="K58" s="5">
+        <f t="shared" si="6"/>
         <v>9.6144601480670588E-5</v>
       </c>
-      <c r="K58" s="1" t="s">
+      <c r="L58" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:12">
       <c r="A59" s="1">
         <v>-4</v>
       </c>
@@ -2943,30 +3060,31 @@
         <v>65</v>
       </c>
       <c r="F59" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.4166666666666661</v>
       </c>
-      <c r="G59" s="3">
+      <c r="G59" s="3"/>
+      <c r="H59" s="3">
         <f t="shared" si="2"/>
         <v>3533</v>
       </c>
-      <c r="H59" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I59" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>DCD</v>
       </c>
-      <c r="I59" s="3">
+      <c r="J59" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333257542</v>
       </c>
-      <c r="J59" s="5">
-        <f t="shared" si="5"/>
+      <c r="K59" s="5">
+        <f t="shared" si="6"/>
         <v>-9.4348523445393555E-5</v>
       </c>
-      <c r="K59" s="1" t="s">
+      <c r="L59" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:12">
       <c r="A60" s="1">
         <v>-3</v>
       </c>
@@ -2985,27 +3103,28 @@
         <v>66</v>
       </c>
       <c r="F60" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.5</v>
       </c>
-      <c r="G60" s="3">
+      <c r="G60" s="3"/>
+      <c r="H60" s="3">
         <f t="shared" si="2"/>
         <v>3600</v>
       </c>
-      <c r="H60" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I60" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>E10</v>
       </c>
-      <c r="I60" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J60" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11">
+      <c r="J60" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K60" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61" s="1">
         <v>-2</v>
       </c>
@@ -3024,30 +3143,31 @@
         <v>67</v>
       </c>
       <c r="F61" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.583333333333333</v>
       </c>
-      <c r="G61" s="3">
+      <c r="G61" s="3"/>
+      <c r="H61" s="3">
         <f t="shared" si="2"/>
         <v>3667</v>
       </c>
-      <c r="H61" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I61" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>E53</v>
       </c>
-      <c r="I61" s="3">
+      <c r="J61" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
-      <c r="J61" s="5">
-        <f t="shared" si="5"/>
+      <c r="K61" s="5">
+        <f t="shared" si="6"/>
         <v>9.0900827197568838E-5</v>
       </c>
-      <c r="K61" s="1" t="s">
+      <c r="L61" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:12">
       <c r="A62" s="1">
         <v>-1</v>
       </c>
@@ -3066,27 +3186,28 @@
         <v>68</v>
       </c>
       <c r="F62" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.6666666666666661</v>
       </c>
-      <c r="G62" s="3">
+      <c r="G62" s="3"/>
+      <c r="H62" s="3">
         <f t="shared" si="2"/>
         <v>3733</v>
       </c>
-      <c r="H62" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I62" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>E95</v>
       </c>
-      <c r="I62" s="3">
+      <c r="J62" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333303017</v>
       </c>
-      <c r="J62" s="5">
-        <f t="shared" si="5"/>
+      <c r="K62" s="5">
+        <f t="shared" si="6"/>
         <v>-8.9293686936252388E-5</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:12">
       <c r="A63" s="1">
         <v>0</v>
       </c>
@@ -3105,30 +3226,31 @@
         <v>69</v>
       </c>
       <c r="F63" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.75</v>
       </c>
-      <c r="G63" s="3">
+      <c r="G63" s="3"/>
+      <c r="H63" s="3">
         <f t="shared" si="2"/>
         <v>3800</v>
       </c>
-      <c r="H63" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I63" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>ED8</v>
       </c>
-      <c r="I63" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J63" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K63" s="1" t="s">
+      <c r="J63" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K63" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L63" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:12">
       <c r="A64" s="1">
         <v>1</v>
       </c>
@@ -3147,27 +3269,28 @@
         <v>70</v>
       </c>
       <c r="F64" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.833333333333333</v>
       </c>
-      <c r="G64" s="3">
+      <c r="G64" s="3"/>
+      <c r="H64" s="3">
         <f t="shared" si="2"/>
         <v>3867</v>
       </c>
-      <c r="H64" s="3" t="str">
-        <f>DEC2HEX(G64,3)</f>
+      <c r="I64" s="3" t="str">
+        <f>DEC2HEX(H64,3)</f>
         <v>F1B</v>
       </c>
-      <c r="I64" s="3">
+      <c r="J64" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333393966</v>
       </c>
-      <c r="J64" s="5">
-        <f t="shared" si="5"/>
+      <c r="K64" s="5">
+        <f t="shared" si="6"/>
         <v>8.6199465563470309E-5</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:12">
       <c r="A65" s="1">
         <v>2</v>
       </c>
@@ -3186,30 +3309,31 @@
         <v>71</v>
       </c>
       <c r="F65" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.9166666666666661</v>
       </c>
-      <c r="G65" s="3">
+      <c r="G65" s="3"/>
+      <c r="H65" s="3">
         <f t="shared" si="2"/>
         <v>3933</v>
       </c>
-      <c r="H65" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I65" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>F5D</v>
       </c>
-      <c r="I65" s="3">
+      <c r="J65" s="3">
         <f t="shared" si="3"/>
         <v>-0.33333333333257542</v>
       </c>
-      <c r="J65" s="5">
-        <f t="shared" si="5"/>
+      <c r="K65" s="5">
+        <f t="shared" si="6"/>
         <v>-8.4752945164651776E-5</v>
       </c>
-      <c r="K65" s="1" t="s">
+      <c r="L65" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:12">
       <c r="A66" s="1">
         <v>3</v>
       </c>
@@ -3228,30 +3352,31 @@
         <v>72</v>
       </c>
       <c r="F66" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="G66" s="3">
+      <c r="G66" s="3"/>
+      <c r="H66" s="3">
         <f t="shared" si="2"/>
         <v>4000</v>
       </c>
-      <c r="H66" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I66" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>FA0</v>
       </c>
-      <c r="I66" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J66" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K66" s="1" t="s">
+      <c r="J66" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K66" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L66" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:12">
       <c r="A67" s="1">
         <v>4</v>
       </c>
@@ -3270,28 +3395,30 @@
         <v>73</v>
       </c>
       <c r="F67" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.083333333333333</v>
       </c>
-      <c r="G67" s="3">
+      <c r="G67" s="3"/>
+      <c r="H67" s="3">
         <f t="shared" si="2"/>
         <v>4067</v>
       </c>
-      <c r="H67" s="3" t="str">
-        <f t="shared" si="4"/>
+      <c r="I67" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>FE3</v>
       </c>
-      <c r="I67" s="3">
+      <c r="J67" s="3">
         <f t="shared" si="3"/>
         <v>0.33333333333348492</v>
       </c>
-      <c r="J67" s="5">
-        <f t="shared" si="5"/>
+      <c r="K67" s="5">
+        <f t="shared" si="6"/>
         <v>8.196049504142732E-5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>